<commit_message>
immer min4 max5 tasks
</commit_message>
<xml_diff>
--- a/Projekte_SCL.xlsx
+++ b/Projekte_SCL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dbsw-my.sharepoint.com/personal/torsten_prigge_deutschebahn_com/Documents/Dokumente/Python/SCL/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_91885D3E39ADF78CDC85D829ED534F09852C6A9D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CEB57D5-21B1-4CC0-AF9D-62320015ED16}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="11_91885D3E39ADF78CDC85D829ED534F09852C6A9D" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB8D21FC-CC45-4BB7-A497-873EA78ABEA4}"/>
   <bookViews>
-    <workbookView xWindow="4755" yWindow="1905" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
   <si>
     <t>Task</t>
   </si>
@@ -49,93 +49,48 @@
     <t>Teko</t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-155  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Deutsches Museum </t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-161 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projekt-162   </t>
-  </si>
-  <si>
     <t>MES</t>
   </si>
   <si>
     <t xml:space="preserve">Allacher Str. </t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-163   </t>
-  </si>
-  <si>
     <t>Citable</t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-168  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Münchenstift Tauernstr. </t>
   </si>
   <si>
     <t xml:space="preserve">Schulcampus Feuerbach </t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-169 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Projekt-170  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Schulcampus Eduard-Stranger </t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-175  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Klinikum Achern </t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-176  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Klinikum Böblingen </t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-179  </t>
-  </si>
-  <si>
     <t xml:space="preserve">MKJZ Westendstraße </t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-182  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Pinakothek </t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-187  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Passauer Straße </t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-169   </t>
-  </si>
-  <si>
     <t>Olympiastadion</t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-190  </t>
-  </si>
-  <si>
     <t xml:space="preserve">Katharinenhospital Stuttgart </t>
   </si>
   <si>
-    <t xml:space="preserve">Projekt-191   </t>
-  </si>
-  <si>
     <t>NGH Herrsching</t>
   </si>
   <si>
@@ -152,6 +107,48 @@
   </si>
   <si>
     <t>Projekt</t>
+  </si>
+  <si>
+    <t>Projekt-155</t>
+  </si>
+  <si>
+    <t>Projekt-161</t>
+  </si>
+  <si>
+    <t>Projekt-162</t>
+  </si>
+  <si>
+    <t>Projekt-163</t>
+  </si>
+  <si>
+    <t>Projekt-168</t>
+  </si>
+  <si>
+    <t>Projekt-169</t>
+  </si>
+  <si>
+    <t>Projekt-170</t>
+  </si>
+  <si>
+    <t>Projekt-175</t>
+  </si>
+  <si>
+    <t>Projekt-176</t>
+  </si>
+  <si>
+    <t>Projekt-179</t>
+  </si>
+  <si>
+    <t>Projekt-182</t>
+  </si>
+  <si>
+    <t>Projekt-187</t>
+  </si>
+  <si>
+    <t>Projekt-190</t>
+  </si>
+  <si>
+    <t>Projekt-191</t>
   </si>
 </sst>
 </file>
@@ -520,8 +517,8 @@
   </sheetPr>
   <dimension ref="A1:B26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -580,138 +577,138 @@
     </row>
     <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
         <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>15</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>